<commit_message>
add web link for every case
</commit_message>
<xml_diff>
--- a/list/UEFI.xlsx
+++ b/list/UEFI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="992"/>
+    <workbookView windowWidth="27690" windowHeight="13350" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="UEFI" sheetId="1" r:id="rId1"/>
@@ -169,11 +169,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="m&quot;／&quot;d&quot;／&quot;yyyy"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="m&quot;／&quot;d&quot;／&quot;yyyy"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -210,8 +210,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,22 +226,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -250,9 +239,44 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,8 +290,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -281,38 +320,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,38 +337,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,6 +354,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,13 +411,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,157 +579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,7 +591,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,6 +755,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -771,10 +801,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -791,33 +819,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -844,142 +845,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
@@ -1021,6 +1022,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1212,10 +1216,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="212121"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F3F3F3"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1471,7 +1475,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -1514,7 +1518,7 @@
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1534,16 +1538,16 @@
       <c r="E2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="24"/>
+      <c r="I2" s="25"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -2568,20 +2572,20 @@
       <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" ht="20" customHeight="1" spans="1:1024">
       <c r="A4" s="8"/>
@@ -2591,20 +2595,20 @@
       <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="24"/>
+      <c r="I4" s="25"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -3629,20 +3633,20 @@
       <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="26"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -4667,20 +4671,20 @@
       <c r="C6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="I6" s="25"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -5707,20 +5711,20 @@
       <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="26"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -6745,20 +6749,20 @@
       <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" ht="20" customHeight="1" spans="1:9">
       <c r="A9" s="8"/>
@@ -6768,20 +6772,20 @@
       <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="25"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="20" customHeight="1" spans="1:9">
       <c r="A10" s="8"/>
@@ -6791,20 +6795,20 @@
       <c r="C10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" ht="20" customHeight="1" spans="1:1024">
       <c r="A11" s="8"/>
@@ -6814,20 +6818,20 @@
       <c r="C11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="25"/>
+      <c r="I11" s="26"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
@@ -7852,20 +7856,20 @@
       <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="25"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -8890,20 +8894,20 @@
       <c r="C13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:9">
       <c r="A14" s="8"/>
@@ -8913,20 +8917,20 @@
       <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" ht="20" customHeight="1" spans="1:9">
       <c r="A15" s="8"/>
@@ -8936,20 +8940,20 @@
       <c r="C15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="25"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" ht="20" customHeight="1" spans="1:9">
       <c r="A16" s="8"/>
@@ -8959,20 +8963,20 @@
       <c r="C16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" ht="20" customHeight="1" spans="1:9">
       <c r="A17" s="8"/>
@@ -8982,20 +8986,20 @@
       <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" ht="20" customHeight="1" spans="1:9">
       <c r="A18" s="8"/>
@@ -9005,20 +9009,20 @@
       <c r="C18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" ht="20" customHeight="1" spans="1:9">
       <c r="A19" s="8"/>
@@ -9028,20 +9032,20 @@
       <c r="C19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="25"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" ht="20" customHeight="1" spans="1:9">
       <c r="A20" s="8" t="s">
@@ -9053,20 +9057,20 @@
       <c r="C20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="24"/>
+      <c r="I20" s="25"/>
     </row>
     <row r="21" ht="20" customHeight="1" spans="1:9">
       <c r="A21" s="8"/>
@@ -9076,20 +9080,20 @@
       <c r="C21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="25"/>
+      <c r="I21" s="26"/>
     </row>
     <row r="22" ht="20" customHeight="1" spans="1:9">
       <c r="A22" s="8"/>
@@ -9099,20 +9103,20 @@
       <c r="C22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="24"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:9">
       <c r="A23" s="8"/>
@@ -9122,23 +9126,23 @@
       <c r="C23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="25"/>
+      <c r="I23" s="26"/>
     </row>
     <row r="24" ht="20" customHeight="1" spans="1:9">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -9147,89 +9151,89 @@
       <c r="C24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="24"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" ht="20" customHeight="1" spans="1:9">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="25"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" ht="20" customHeight="1" spans="1:9">
-      <c r="A26" s="14"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="24"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" ht="20" customHeight="1" spans="1:9">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="26"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" ht="14.65" customHeight="1"/>
     <row r="29" ht="14.65" customHeight="1"/>
@@ -9273,6 +9277,7 @@
     <hyperlink ref="D20" r:id="rId1"/>
     <hyperlink ref="D24" r:id="rId1"/>
     <hyperlink ref="D2:D6" r:id="rId1" display="UEFI.md"/>
+    <hyperlink ref="D2:D27" r:id="rId2" display="UEFI.md"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>